<commit_message>
Implemented YouTube data fetcher to retrieve videos and comments from a channel. - Added functionality to fetch channel ID and name using YouTube API. - Extracted video details including views, likes, and comments. - Exported video data and comments to an Excel file with dynamic filename based on channel name. - Added input validation for YouTube channel URL.
</commit_message>
<xml_diff>
--- a/output/YouTube_Cricket Majestic.xlsx
+++ b/output/YouTube_Cricket Majestic.xlsx
@@ -543,7 +543,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>13378</t>
+          <t>13513</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>21893</t>
+          <t>21939</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -629,12 +629,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>60194</t>
+          <t>60305</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>956</t>
+          <t>959</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -672,7 +672,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>594</t>
+          <t>600</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -715,12 +715,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>24345</t>
+          <t>24426</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>351</t>
+          <t>350</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -844,7 +844,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5009</t>
+          <t>5022</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -887,12 +887,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>55900</t>
+          <t>55945</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>610</t>
+          <t>611</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -930,12 +930,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>892741</t>
+          <t>894149</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>8836</t>
+          <t>8840</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -973,7 +973,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1272</t>
+          <t>1279</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
@@ -7091,7 +7091,7 @@
         </is>
       </c>
       <c r="F190" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G190" t="inlineStr"/>
     </row>

</xml_diff>